<commit_message>
Add IPO dates for airlines
</commit_message>
<xml_diff>
--- a/$ATSG.xlsx
+++ b/$ATSG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EE72A4-FA69-4EBE-B619-BF3D06CED563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5DCA23-6329-4EDD-8D54-518047801CE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{51E7658F-16C5-4CFF-B191-0B4CB4BA3BCF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{51E7658F-16C5-4CFF-B191-0B4CB4BA3BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
   <si>
     <t>$ATSG</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>Share Price</t>
+  </si>
+  <si>
+    <t>IPO</t>
+  </si>
+  <si>
+    <t>(Formerly ABX Air)</t>
   </si>
 </sst>
 </file>
@@ -504,8 +510,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0\x"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -716,63 +722,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,12 +749,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -818,8 +781,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -845,16 +808,59 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1343,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB32BC0B-91D8-4B9D-B35A-9988AB593C97}">
   <dimension ref="A2:AA41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1363,780 +1369,784 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="I5" s="3" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="I5" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="5"/>
-      <c r="X5" s="3" t="s">
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="49"/>
+      <c r="X5" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="5"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="49"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>28.47</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="19"/>
-      <c r="X6" s="60" t="s">
+      <c r="D6" s="11"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="10"/>
+      <c r="X6" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="19"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="10"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="13">
         <f>'Financial Model'!T32</f>
         <v>73.98</v>
       </c>
-      <c r="D7" s="26" t="str">
+      <c r="D7" s="11" t="str">
         <f>$C$33</f>
         <v>Q222</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="19"/>
-      <c r="X7" s="61"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="19"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="10"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="10"/>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="13">
         <f>C6*C7</f>
         <v>2106.2105999999999</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="19"/>
-      <c r="X8" s="60" t="s">
+      <c r="D8" s="11"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="10"/>
+      <c r="X8" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="19"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="10"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="13">
         <f>'Financial Model'!T78</f>
         <v>47.151000000000003</v>
       </c>
-      <c r="D9" s="26" t="str">
+      <c r="D9" s="11" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$33</f>
         <v>Q222</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="19"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="19"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="10"/>
+      <c r="X9" s="43"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="10"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="13">
         <f>'Financial Model'!T79</f>
         <v>1359.4760000000001</v>
       </c>
-      <c r="D10" s="26" t="str">
+      <c r="D10" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Q222</v>
       </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="19"/>
-      <c r="X10" s="60" t="s">
+      <c r="I10" s="41"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="10"/>
+      <c r="X10" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="19"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="10"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="13">
         <f>C9-C10</f>
         <v>-1312.325</v>
       </c>
-      <c r="D11" s="26" t="str">
+      <c r="D11" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Q222</v>
       </c>
-      <c r="I11" s="58"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="19"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="19"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="10"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="10"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="14">
         <f>C8-C11</f>
         <v>3418.5356000000002</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="19"/>
-      <c r="X12" s="60" t="s">
+      <c r="D12" s="12"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="10"/>
+      <c r="X12" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="19"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="10"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="I13" s="58"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="19"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30"/>
-      <c r="AA13" s="19"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="10"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="I14" s="58"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="19"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="30"/>
-      <c r="AA14" s="19"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="10"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="19"/>
-      <c r="X15" s="60"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="19"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="10"/>
+      <c r="X15" s="43"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="19"/>
-      <c r="X16" s="60"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="30"/>
-      <c r="AA16" s="19"/>
+      <c r="D16" s="63"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="10"/>
+      <c r="X16" s="43"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="19"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="30"/>
-      <c r="AA17" s="19"/>
+      <c r="D17" s="63"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="10"/>
+      <c r="X17" s="43"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="19"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="19"/>
+      <c r="D18" s="63"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="10"/>
+      <c r="X18" s="43"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="19"/>
-      <c r="X19" s="60"/>
-      <c r="Y19" s="30"/>
-      <c r="Z19" s="30"/>
-      <c r="AA19" s="19"/>
+      <c r="D19" s="65"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="10"/>
+      <c r="X19" s="43"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="10"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I20" s="58"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="19"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="10"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I21" s="58"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="19"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="10"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="19"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="10"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="32">
+      <c r="C23" s="59"/>
+      <c r="D23" s="17">
         <v>117</v>
       </c>
-      <c r="I23" s="58"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="19"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="10"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="32">
+      <c r="C24" s="59"/>
+      <c r="D24" s="17">
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="58"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="19"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="10"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="53" t="s">
+      <c r="C25" s="61"/>
+      <c r="D25" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="58"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="19"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="10"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I26" s="58"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="19"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="10"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I27" s="58"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="19"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="10"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="19"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="10"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="19"/>
+      <c r="D29" s="63"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="10"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="33">
+      <c r="C30" s="62">
         <v>1980</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="19"/>
+      <c r="D30" s="63"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="10"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="13"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="19"/>
+      <c r="B31" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="62">
+        <v>2003</v>
+      </c>
+      <c r="D31" s="63"/>
+      <c r="E31" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="41"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="10"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B32" s="13"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="19"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="10"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="55">
+      <c r="D33" s="38">
         <v>44777</v>
       </c>
-      <c r="I33" s="58"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="19"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="10"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
-      <c r="V34" s="16"/>
+      <c r="D34" s="57"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="9"/>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="62">
+      <c r="C38" s="50">
         <f>C6/'Financial Model'!T76</f>
         <v>1.4921863586996182</v>
       </c>
-      <c r="D38" s="63"/>
+      <c r="D38" s="51"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="53"/>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="X5:AA5"/>
     <mergeCell ref="I5:V5"/>
     <mergeCell ref="C32:D32"/>
@@ -2153,8 +2163,11 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{0836D631-5ACB-4443-AB96-A775C04443E2}"/>
@@ -2170,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA568596-2CBE-4605-B6B1-4152BAAFA3C8}">
   <dimension ref="A1:BB89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AC10" sqref="AC10"/>
@@ -2184,171 +2197,171 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="1:54" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="W1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="X1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="35" t="s">
+      <c r="Y1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="Z1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="35" t="s">
+      <c r="AC1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AD1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AE1" s="35" t="s">
+      <c r="AE1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AF1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AG1" s="35" t="s">
+      <c r="AG1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AH1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="35" t="s">
+      <c r="AI1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="35" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AK1" s="35" t="s">
+      <c r="AK1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AL1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="35" t="s">
+      <c r="AM1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="35" t="s">
+      <c r="AN1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="AO1" s="35" t="s">
+      <c r="AO1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AP1" s="35" t="s">
+      <c r="AP1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="AQ1" s="35" t="s">
+      <c r="AQ1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AR1" s="35" t="s">
+      <c r="AR1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AS1" s="35" t="s">
+      <c r="AS1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AT1" s="35" t="s">
+      <c r="AT1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AU1" s="35" t="s">
+      <c r="AU1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="AV1" s="35" t="s">
+      <c r="AV1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="AW1" s="35" t="s">
+      <c r="AW1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AX1" s="35" t="s">
+      <c r="AX1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AY1" s="35" t="s">
+      <c r="AY1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="35" t="s">
+      <c r="AZ1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="BA1" s="35" t="s">
+      <c r="BA1" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="BB1" s="35" t="s">
+      <c r="BB1" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36"/>
-      <c r="P2" s="42">
+    <row r="2" spans="1:54" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="19"/>
+      <c r="P2" s="25">
         <v>44377</v>
       </c>
-      <c r="T2" s="42">
+      <c r="T2" s="25">
         <v>44742</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="T3" s="54">
+    <row r="3" spans="1:54" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="T3" s="37">
         <v>38200</v>
       </c>
     </row>
@@ -2356,125 +2369,125 @@
       <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="31">
         <v>409.87200000000001</v>
       </c>
-      <c r="T4" s="48">
+      <c r="T4" s="31">
         <v>509.66800000000001</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="30">
         <v>141.524</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="30">
         <v>162.797</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="P6" s="47">
+      <c r="P6" s="30">
         <v>45.912999999999997</v>
       </c>
-      <c r="T6" s="47">
+      <c r="T6" s="30">
         <v>39.406999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="47">
+      <c r="P7" s="30">
         <v>36.591999999999999</v>
       </c>
-      <c r="T7" s="47">
+      <c r="T7" s="30">
         <v>73.102000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="30">
         <v>18.794</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="30">
         <v>20.152999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="P9" s="47">
+      <c r="P9" s="30">
         <v>18.501000000000001</v>
       </c>
-      <c r="T9" s="47">
+      <c r="T9" s="30">
         <v>28.48</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="P10" s="47">
+      <c r="P10" s="30">
         <v>3.0259999999999998</v>
       </c>
-      <c r="T10" s="47">
+      <c r="T10" s="30">
         <v>4.085</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="P11" s="47">
+      <c r="P11" s="30">
         <v>5.726</v>
       </c>
-      <c r="T11" s="47">
+      <c r="T11" s="30">
         <v>7.0679999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="P12" s="47">
+      <c r="P12" s="30">
         <v>3.0680000000000001</v>
       </c>
-      <c r="T12" s="47">
+      <c r="T12" s="30">
         <v>2.3260000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="30">
         <f>SUM(P5:P12)</f>
         <v>273.14400000000001</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="30">
         <f>SUM(T5:T12)</f>
         <v>337.41800000000006</v>
       </c>
     </row>
     <row r="14" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="P14" s="48">
+      <c r="P14" s="31">
         <f>P4-P13</f>
         <v>136.72800000000001</v>
       </c>
-      <c r="T14" s="48">
+      <c r="T14" s="31">
         <f>T4-T13</f>
         <v>172.24999999999994</v>
       </c>
@@ -2484,10 +2497,10 @@
       <c r="B15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="30">
         <v>75.632999999999996</v>
       </c>
-      <c r="T15" s="47">
+      <c r="T15" s="30">
         <v>81.372</v>
       </c>
     </row>
@@ -2495,10 +2508,10 @@
       <c r="B16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="47">
+      <c r="P16" s="30">
         <v>14.75</v>
       </c>
-      <c r="T16" s="47">
+      <c r="T16" s="30">
         <v>20.361000000000001</v>
       </c>
     </row>
@@ -2506,10 +2519,10 @@
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P17" s="47">
+      <c r="P17" s="30">
         <v>38.274000000000001</v>
       </c>
-      <c r="T17" s="47">
+      <c r="T17" s="30">
         <v>0</v>
       </c>
     </row>
@@ -2517,11 +2530,11 @@
       <c r="B18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P18" s="48">
+      <c r="P18" s="31">
         <f>P14-P15-P16+P17</f>
         <v>84.619000000000014</v>
       </c>
-      <c r="T18" s="48">
+      <c r="T18" s="31">
         <f>T14-T15-T16+T17</f>
         <v>70.516999999999939</v>
       </c>
@@ -2531,7 +2544,7 @@
       <c r="B19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P19" s="47">
+      <c r="P19" s="30">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="T19" s="2">
@@ -2542,7 +2555,7 @@
       <c r="B20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P20" s="47">
+      <c r="P20" s="30">
         <v>4.4560000000000004</v>
       </c>
       <c r="T20" s="2">
@@ -2553,7 +2566,7 @@
       <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P21" s="47">
+      <c r="P21" s="30">
         <v>-6.5049999999999999</v>
       </c>
       <c r="T21" s="2">
@@ -2564,7 +2577,7 @@
       <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="P22" s="47">
+      <c r="P22" s="30">
         <v>35.703000000000003</v>
       </c>
       <c r="T22" s="2">
@@ -2576,7 +2589,7 @@
       <c r="B23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="P23" s="47">
+      <c r="P23" s="30">
         <v>0.96499999999999997</v>
       </c>
       <c r="T23" s="2">
@@ -2588,7 +2601,7 @@
       <c r="B24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="P24" s="47">
+      <c r="P24" s="30">
         <v>-15.021000000000001</v>
       </c>
       <c r="T24" s="2">
@@ -2600,7 +2613,7 @@
       <c r="B25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="P25" s="47">
+      <c r="P25" s="30">
         <f>P19+P20+P21+P22+P23+P24</f>
         <v>19.607000000000006</v>
       </c>
@@ -2613,11 +2626,11 @@
       <c r="B26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="P26" s="47">
+      <c r="P26" s="30">
         <f>P18+P25</f>
         <v>104.22600000000003</v>
       </c>
-      <c r="T26" s="47">
+      <c r="T26" s="30">
         <f>T18+T25</f>
         <v>69.249999999999943</v>
       </c>
@@ -2626,7 +2639,7 @@
       <c r="B27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="P27" s="47">
+      <c r="P27" s="30">
         <v>24.356999999999999</v>
       </c>
       <c r="T27" s="2">
@@ -2637,11 +2650,11 @@
       <c r="B28" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="P28" s="47">
+      <c r="P28" s="30">
         <f>P26-P27</f>
         <v>79.869000000000028</v>
       </c>
-      <c r="T28" s="47">
+      <c r="T28" s="30">
         <f>T26-T27</f>
         <v>54.209999999999944</v>
       </c>
@@ -2650,7 +2663,7 @@
       <c r="B29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="P29" s="47">
+      <c r="P29" s="30">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="T29" s="2">
@@ -2661,11 +2674,11 @@
       <c r="B30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="P30" s="48">
+      <c r="P30" s="31">
         <f>P28+P29</f>
         <v>79.934000000000026</v>
       </c>
-      <c r="T30" s="48">
+      <c r="T30" s="31">
         <f>T28+T29</f>
         <v>55.091999999999942</v>
       </c>
@@ -2674,11 +2687,11 @@
       <c r="B31" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P31" s="49">
+      <c r="P31" s="32">
         <f>P30/P32</f>
         <v>1.1719496818461723</v>
       </c>
-      <c r="T31" s="49">
+      <c r="T31" s="32">
         <f>T30/T32</f>
         <v>0.74468775344687665</v>
       </c>
@@ -2695,11 +2708,11 @@
       </c>
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="43"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="T34" s="51">
+      <c r="T34" s="34">
         <f>T4/P4-1</f>
         <v>0.24348089159542496</v>
       </c>
@@ -2713,39 +2726,39 @@
       <c r="B37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="P37" s="50">
+      <c r="P37" s="33">
         <f>P14/P4</f>
         <v>0.3335870710856072</v>
       </c>
-      <c r="T37" s="50">
+      <c r="T37" s="33">
         <f>T14/T4</f>
         <v>0.33796510669690843</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P38" s="50">
+      <c r="P38" s="33">
         <f>P18/P4</f>
         <v>0.20645225826599525</v>
       </c>
-      <c r="T38" s="50">
+      <c r="T38" s="33">
         <f>T18/T4</f>
         <v>0.13835869624932295</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="P39" s="50">
+      <c r="P39" s="33">
         <f>P30/P4</f>
         <v>0.19502186048327289</v>
       </c>
-      <c r="T39" s="50">
+      <c r="T39" s="33">
         <f>T30/T4</f>
         <v>0.10809389641884509</v>
       </c>
@@ -2754,20 +2767,20 @@
       <c r="B40" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="P40" s="50">
+      <c r="P40" s="33">
         <f>P27/P26</f>
         <v>0.23369408784756196</v>
       </c>
-      <c r="T40" s="50">
+      <c r="T40" s="33">
         <f>T27/T26</f>
         <v>0.21718411552346586</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
+      <c r="A41" s="20"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="35" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2775,7 +2788,7 @@
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T45" s="48">
+      <c r="T45" s="31">
         <v>47.151000000000003</v>
       </c>
     </row>
@@ -2784,7 +2797,7 @@
       <c r="B46" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="T46" s="47">
+      <c r="T46" s="30">
         <v>260.26</v>
       </c>
     </row>
@@ -2793,7 +2806,7 @@
       <c r="B47" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="T47" s="47">
+      <c r="T47" s="30">
         <v>54.005000000000003</v>
       </c>
     </row>
@@ -2801,7 +2814,7 @@
       <c r="B48" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="T48" s="47">
+      <c r="T48" s="30">
         <v>28.157</v>
       </c>
     </row>
@@ -2809,7 +2822,7 @@
       <c r="B49" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="T49" s="47">
+      <c r="T49" s="30">
         <f>SUM(T45:T48)</f>
         <v>389.57299999999998</v>
       </c>
@@ -2818,7 +2831,7 @@
       <c r="B50" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="T50" s="47">
+      <c r="T50" s="30">
         <v>2270.6559999999999</v>
       </c>
     </row>
@@ -2826,7 +2839,7 @@
       <c r="B51" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="T51" s="47">
+      <c r="T51" s="30">
         <v>91.293000000000006</v>
       </c>
     </row>
@@ -2834,7 +2847,7 @@
       <c r="B52" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T52" s="47">
+      <c r="T52" s="30">
         <v>498.07299999999998</v>
       </c>
     </row>
@@ -2842,7 +2855,7 @@
       <c r="B53" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="T53" s="47">
+      <c r="T53" s="30">
         <v>64.155000000000001</v>
       </c>
     </row>
@@ -2850,7 +2863,7 @@
       <c r="B54" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="T54" s="47">
+      <c r="T54" s="30">
         <v>145.80000000000001</v>
       </c>
     </row>
@@ -2858,19 +2871,19 @@
       <c r="B55" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="T55" s="47">
+      <c r="T55" s="30">
         <f>T49+SUM(T50:T54)</f>
         <v>3459.55</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="T56" s="47"/>
+      <c r="T56" s="30"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="T57" s="47">
+      <c r="T57" s="30">
         <v>194.95099999999999</v>
       </c>
     </row>
@@ -2878,7 +2891,7 @@
       <c r="B58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="T58" s="47">
+      <c r="T58" s="30">
         <v>62.537999999999997</v>
       </c>
     </row>
@@ -2886,7 +2899,7 @@
       <c r="B59" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="T59" s="47">
+      <c r="T59" s="30">
         <v>11.423</v>
       </c>
     </row>
@@ -2894,7 +2907,7 @@
       <c r="B60" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="T60" s="48">
+      <c r="T60" s="31">
         <v>0.63400000000000001</v>
       </c>
     </row>
@@ -2902,7 +2915,7 @@
       <c r="B61" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T61" s="47">
+      <c r="T61" s="30">
         <v>20.497</v>
       </c>
     </row>
@@ -2910,7 +2923,7 @@
       <c r="B62" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T62" s="47">
+      <c r="T62" s="30">
         <v>38.292999999999999</v>
       </c>
     </row>
@@ -2918,7 +2931,7 @@
       <c r="B63" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="T63" s="47">
+      <c r="T63" s="30">
         <f>SUM(T57:T62)</f>
         <v>328.33600000000001</v>
       </c>
@@ -2927,7 +2940,7 @@
       <c r="B64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="T64" s="48">
+      <c r="T64" s="31">
         <v>1358.8420000000001</v>
       </c>
     </row>
@@ -2936,7 +2949,7 @@
       <c r="B65" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="T65" s="47">
+      <c r="T65" s="30">
         <v>0.85099999999999998</v>
       </c>
     </row>
@@ -2945,7 +2958,7 @@
       <c r="B66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="T66" s="47">
+      <c r="T66" s="30">
         <v>20.375</v>
       </c>
     </row>
@@ -2953,7 +2966,7 @@
       <c r="B67" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="T67" s="47">
+      <c r="T67" s="30">
         <v>44.305</v>
       </c>
     </row>
@@ -2961,7 +2974,7 @@
       <c r="B68" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="T68" s="47">
+      <c r="T68" s="30">
         <v>53.595999999999997</v>
       </c>
     </row>
@@ -2969,7 +2982,7 @@
       <c r="B69" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="T69" s="47">
+      <c r="T69" s="30">
         <v>241.75200000000001</v>
       </c>
     </row>
@@ -2977,7 +2990,7 @@
       <c r="B70" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="T70" s="47">
+      <c r="T70" s="30">
         <f>T63+SUM(T64:T69)</f>
         <v>2048.0570000000002</v>
       </c>
@@ -2986,7 +2999,7 @@
       <c r="B72" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="T72" s="47">
+      <c r="T72" s="30">
         <v>1411.4929999999999</v>
       </c>
     </row>
@@ -2994,7 +3007,7 @@
       <c r="B73" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="T73" s="47">
+      <c r="T73" s="30">
         <f>T72+T70</f>
         <v>3459.55</v>
       </c>
@@ -3003,13 +3016,13 @@
       <c r="B75" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="T75" s="47">
+      <c r="T75" s="30">
         <f>T55-T70</f>
         <v>1411.4929999999999</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="2" t="s">
         <v>155</v>
       </c>
@@ -3019,22 +3032,22 @@
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-    </row>
-    <row r="78" spans="1:20" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="37" t="s">
+      <c r="A77" s="20"/>
+    </row>
+    <row r="78" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="T78" s="65">
+      <c r="T78" s="46">
         <f>T45</f>
         <v>47.151000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:20" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="37" t="s">
+    <row r="79" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="T79" s="65">
+      <c r="T79" s="46">
         <f>T60+T64</f>
         <v>1359.4760000000001</v>
       </c>
@@ -3043,7 +3056,7 @@
       <c r="B80" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="T80" s="47">
+      <c r="T80" s="30">
         <f>T78-T79</f>
         <v>-1312.325</v>
       </c>
@@ -3060,7 +3073,7 @@
       <c r="B83" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T83" s="47">
+      <c r="T83" s="30">
         <f>T82*T32</f>
         <v>2125.4454000000001</v>
       </c>
@@ -3069,7 +3082,7 @@
       <c r="B84" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="T84" s="47">
+      <c r="T84" s="30">
         <f>T83-T80</f>
         <v>3437.7704000000003</v>
       </c>
@@ -3078,7 +3091,7 @@
       <c r="B86" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T86" s="64">
+      <c r="T86" s="45">
         <f>T82/T76</f>
         <v>1.5058136313818067</v>
       </c>

</xml_diff>

<commit_message>
$ATSG Q322/21 financial data
</commit_message>
<xml_diff>
--- a/$ATSG.xlsx
+++ b/$ATSG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5DCA23-6329-4EDD-8D54-518047801CE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21FC029-24D2-8241-B33E-4FCD2EE6798E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{51E7658F-16C5-4CFF-B191-0B4CB4BA3BCF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{51E7658F-16C5-4CFF-B191-0B4CB4BA3BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="170">
   <si>
     <t>$ATSG</t>
   </si>
@@ -406,12 +416,6 @@
     <t>Primary US DoD Contractor</t>
   </si>
   <si>
-    <t>Omani Air</t>
-  </si>
-  <si>
-    <t>Prime Air</t>
-  </si>
-  <si>
     <t>A/R</t>
   </si>
   <si>
@@ -503,6 +507,45 @@
   </si>
   <si>
     <t>(Formerly ABX Air)</t>
+  </si>
+  <si>
+    <t>ATSG &amp; GA Telesis announced a joint-venture that will establish an engine hospital facility in the United States</t>
+  </si>
+  <si>
+    <t>ATSG announced it was to acquire Omni Air International based in Tulsa, Oklahoma - a passenger &amp; charter services specialised in serving US &amp; foreign Govt.</t>
+  </si>
+  <si>
+    <t>Subsidiaries</t>
+  </si>
+  <si>
+    <t>Cargo Aircraft Management</t>
+  </si>
+  <si>
+    <t>Airborne Global Solutions</t>
+  </si>
+  <si>
+    <t>Air Transport International (Cargo &amp; Pax)</t>
+  </si>
+  <si>
+    <t>ABX Air (Cargo Airline)</t>
+  </si>
+  <si>
+    <t>Omni Air International (Pax leasing, Charter)</t>
+  </si>
+  <si>
+    <t>Airborne Maintenance &amp; Engineering Services</t>
+  </si>
+  <si>
+    <t>PEMCO Conversions (737 &amp; A321 to freight)</t>
+  </si>
+  <si>
+    <t>LGSTX Services (Airport Support Services)</t>
+  </si>
+  <si>
+    <t>TriFactor Distribution Solutions</t>
+  </si>
+  <si>
+    <t>Retired 40yr CEO (2020)</t>
   </si>
 </sst>
 </file>
@@ -513,7 +556,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,8 +641,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +671,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -802,8 +858,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -812,25 +866,39 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -849,18 +917,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -942,6 +1019,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>132466</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E629C1CE-CB85-EF29-4B9C-530060480261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6299200" y="5816600"/>
+          <a:ext cx="7467600" cy="3066166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -949,13 +1070,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>98</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -973,8 +1094,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13639800" y="0"/>
-          <a:ext cx="0" cy="15954375"/>
+          <a:off x="16316325" y="0"/>
+          <a:ext cx="0" cy="16278225"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1350,54 +1471,55 @@
   <dimension ref="A2:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="47" t="s">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B5" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="I5" s="47" t="s">
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
+      <c r="H5" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="49"/>
-      <c r="X5" s="47" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="57"/>
+      <c r="X5" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="49"/>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="57"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1405,7 +1527,8 @@
         <v>28.47</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="I6" s="41"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -1419,26 +1542,27 @@
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
       <c r="V6" s="10"/>
-      <c r="X6" s="43" t="s">
+      <c r="X6" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="10"/>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="46"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="13">
-        <f>'Financial Model'!T32</f>
-        <v>73.98</v>
+        <f>'Financial Model'!U32</f>
+        <v>73.998000000000005</v>
       </c>
       <c r="D7" s="11" t="str">
         <f>$C$33</f>
-        <v>Q222</v>
-      </c>
-      <c r="I7" s="41"/>
+        <v>Q322</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -1452,21 +1576,22 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="10"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="10"/>
-    </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X7" s="42"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="46"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="13">
         <f>C6*C7</f>
-        <v>2106.2105999999999</v>
+        <v>2106.7230600000003</v>
       </c>
       <c r="D8" s="11"/>
-      <c r="I8" s="41"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -1480,26 +1605,27 @@
       <c r="T8" s="15"/>
       <c r="U8" s="15"/>
       <c r="V8" s="10"/>
-      <c r="X8" s="43" t="s">
+      <c r="X8" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="10"/>
-    </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="45"/>
+      <c r="AA8" s="46"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13">
-        <f>'Financial Model'!T78</f>
-        <v>47.151000000000003</v>
+        <f>'Financial Model'!U78</f>
+        <v>54.485999999999997</v>
       </c>
       <c r="D9" s="11" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$33</f>
-        <v>Q222</v>
-      </c>
-      <c r="I9" s="41"/>
+        <v>Q322</v>
+      </c>
+      <c r="H9" s="49"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -1513,24 +1639,25 @@
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
       <c r="V9" s="10"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="10"/>
-    </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X9" s="41"/>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="46"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="13">
-        <f>'Financial Model'!T79</f>
-        <v>1359.4760000000001</v>
+        <f>'Financial Model'!U79</f>
+        <v>1369.643</v>
       </c>
       <c r="D10" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Q222</v>
-      </c>
-      <c r="I10" s="41"/>
+        <v>Q322</v>
+      </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
@@ -1544,26 +1671,25 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="10"/>
-      <c r="X10" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="10"/>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X10" s="41"/>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="45"/>
+      <c r="AA10" s="46"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="13">
         <f>C9-C10</f>
-        <v>-1312.325</v>
+        <v>-1315.1569999999999</v>
       </c>
       <c r="D11" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Q222</v>
-      </c>
-      <c r="I11" s="41"/>
+        <v>Q322</v>
+      </c>
+      <c r="H11" s="49"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1577,21 +1703,24 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="10"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="10"/>
-    </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X11" s="72" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="46"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="14">
         <f>C8-C11</f>
-        <v>3418.5356000000002</v>
+        <v>3421.8800600000004</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="I12" s="41"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -1605,15 +1734,16 @@
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
       <c r="V12" s="10"/>
-      <c r="X12" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="10"/>
-    </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="I13" s="41"/>
+      <c r="X12" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="46"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="H13" s="49"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -1627,13 +1757,16 @@
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
       <c r="V13" s="10"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="10"/>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="I14" s="41"/>
+      <c r="X13" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="46"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="H14" s="49"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
@@ -1647,18 +1780,21 @@
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
       <c r="V14" s="10"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="10"/>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="47" t="s">
+      <c r="X14" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="46"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B15" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="I15" s="41"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
@@ -1672,20 +1808,23 @@
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
       <c r="V15" s="10"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="10"/>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X15" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="46"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B16" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="I16" s="41"/>
+      <c r="D16" s="52"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
@@ -1699,20 +1838,27 @@
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
       <c r="V16" s="10"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="10"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X16" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="46"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B17" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="I17" s="41"/>
+      <c r="D17" s="52"/>
+      <c r="H17" s="71">
+        <v>44317</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>157</v>
+      </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
@@ -1726,20 +1872,23 @@
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
       <c r="V17" s="10"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="10"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X17" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
+      <c r="AA17" s="46"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B18" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="I18" s="41"/>
+      <c r="D18" s="52"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
@@ -1753,20 +1902,27 @@
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
       <c r="V18" s="10"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="10"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X18" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="46"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A19" s="73"/>
       <c r="B19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="I19" s="41"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="49"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
@@ -1780,13 +1936,16 @@
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
       <c r="V19" s="10"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="10"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I20" s="41"/>
+      <c r="X19" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="46"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="H20" s="49"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
@@ -1800,9 +1959,16 @@
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
       <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I21" s="41"/>
+      <c r="X20" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="46"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="H21" s="49"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
@@ -1816,14 +1982,19 @@
       <c r="T21" s="15"/>
       <c r="U21" s="15"/>
       <c r="V21" s="10"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="47" t="s">
+      <c r="X21" s="41"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="45"/>
+      <c r="AA21" s="46"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B22" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="I22" s="41"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
@@ -1837,19 +2008,24 @@
       <c r="T22" s="15"/>
       <c r="U22" s="15"/>
       <c r="V22" s="10"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X22" s="74"/>
+      <c r="Y22" s="47"/>
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="48"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="17">
         <v>117</v>
       </c>
-      <c r="I23" s="41"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="45"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -1864,18 +2040,19 @@
       <c r="U23" s="15"/>
       <c r="V23" s="10"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="58" t="s">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B24" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="59"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="17">
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="41"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="45"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
@@ -1890,15 +2067,16 @@
       <c r="U24" s="15"/>
       <c r="V24" s="10"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="60" t="s">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B25" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="61"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="41"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="45"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
@@ -1913,8 +2091,9 @@
       <c r="U25" s="15"/>
       <c r="V25" s="10"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I26" s="41"/>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="H26" s="49"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
@@ -1929,8 +2108,9 @@
       <c r="U26" s="15"/>
       <c r="V26" s="10"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I27" s="41"/>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="H27" s="49"/>
+      <c r="I27" s="45"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
@@ -1945,13 +2125,18 @@
       <c r="U27" s="15"/>
       <c r="V27" s="10"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B28" s="47" t="s">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B28" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="I28" s="41"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="H28" s="71">
+        <v>43374</v>
+      </c>
+      <c r="I28" s="45" t="s">
+        <v>158</v>
+      </c>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
@@ -1966,15 +2151,16 @@
       <c r="U28" s="15"/>
       <c r="V28" s="10"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="63"/>
-      <c r="I29" s="41"/>
+      <c r="D29" s="52"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="45"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
@@ -1989,15 +2175,16 @@
       <c r="U29" s="15"/>
       <c r="V29" s="10"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="62">
+      <c r="C30" s="51">
         <v>1980</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="I30" s="41"/>
+      <c r="D30" s="52"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="45"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
@@ -2012,18 +2199,19 @@
       <c r="U30" s="15"/>
       <c r="V30" s="10"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B31" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" s="62">
+        <v>155</v>
+      </c>
+      <c r="C31" s="51">
         <v>2003</v>
       </c>
-      <c r="D31" s="63"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I31" s="41"/>
+        <v>156</v>
+      </c>
+      <c r="H31" s="49"/>
+      <c r="I31" s="45"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
@@ -2038,11 +2226,12 @@
       <c r="U31" s="15"/>
       <c r="V31" s="10"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B32" s="6"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="53"/>
-      <c r="I32" s="41"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="45"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
@@ -2057,17 +2246,18 @@
       <c r="U32" s="15"/>
       <c r="V32" s="10"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D33" s="38">
-        <v>44777</v>
-      </c>
-      <c r="I33" s="41"/>
+        <v>44868</v>
+      </c>
+      <c r="H33" s="49"/>
+      <c r="I33" s="45"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
@@ -2082,15 +2272,16 @@
       <c r="U33" s="15"/>
       <c r="V33" s="10"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="57"/>
-      <c r="I34" s="42"/>
+      <c r="D34" s="61"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -2105,51 +2296,51 @@
       <c r="U34" s="8"/>
       <c r="V34" s="9"/>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="B37" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
-    </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="50">
-        <f>C6/'Financial Model'!T76</f>
-        <v>1.4921863586996182</v>
-      </c>
-      <c r="D38" s="51"/>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C38" s="66">
+        <f>C6/'Financial Model'!U76</f>
+        <v>1.4375141996217067</v>
+      </c>
+      <c r="D38" s="67"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C39" s="58"/>
+      <c r="D39" s="59"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53"/>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C40" s="58"/>
+      <c r="D40" s="59"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="55"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="I5:V5"/>
-    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -2159,15 +2350,15 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="H5:V5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{0836D631-5ACB-4443-AB96-A775C04443E2}"/>
@@ -2184,20 +2375,20 @@
   <dimension ref="A1:BB89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AC10" sqref="AC10"/>
+      <selection pane="bottomRight" activeCell="U86" sqref="U86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="C1" s="18" t="s">
         <v>31</v>
       </c>
@@ -2252,7 +2443,7 @@
       <c r="T1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="75" t="s">
         <v>49</v>
       </c>
       <c r="V1" s="18" t="s">
@@ -2349,111 +2540,171 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="19"/>
       <c r="P2" s="25">
         <v>44377</v>
       </c>
+      <c r="Q2" s="25">
+        <v>44469</v>
+      </c>
+      <c r="R2" s="25">
+        <v>44561</v>
+      </c>
       <c r="T2" s="25">
         <v>44742</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U2" s="25">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="T3" s="37">
         <v>38200</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U3" s="37">
+        <v>37926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
       <c r="P4" s="31">
         <v>409.87200000000001</v>
       </c>
+      <c r="Q4" s="31">
+        <v>465.95499999999998</v>
+      </c>
       <c r="T4" s="31">
         <v>509.66800000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U4" s="31">
+        <v>516.91600000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B5" s="27" t="s">
         <v>82</v>
       </c>
       <c r="P5" s="30">
         <v>141.524</v>
       </c>
+      <c r="Q5" s="30">
+        <v>148.07400000000001</v>
+      </c>
       <c r="T5" s="30">
         <v>162.797</v>
       </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U5" s="30">
+        <v>169.96700000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B6" s="27" t="s">
         <v>84</v>
       </c>
       <c r="P6" s="30">
         <v>45.912999999999997</v>
       </c>
+      <c r="Q6" s="30">
+        <v>43.750999999999998</v>
+      </c>
       <c r="T6" s="30">
         <v>39.406999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U6" s="30">
+        <v>41.540999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B7" s="27" t="s">
         <v>85</v>
       </c>
       <c r="P7" s="30">
         <v>36.591999999999999</v>
       </c>
+      <c r="Q7" s="30">
+        <v>50.176000000000002</v>
+      </c>
       <c r="T7" s="30">
         <v>73.102000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U7" s="30">
+        <v>68.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
       <c r="P8" s="30">
         <v>18.794</v>
       </c>
+      <c r="Q8" s="30">
+        <v>21.62</v>
+      </c>
       <c r="T8" s="30">
         <v>20.152999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U8" s="30">
+        <v>18.277999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B9" s="27" t="s">
         <v>87</v>
       </c>
       <c r="P9" s="30">
         <v>18.501000000000001</v>
       </c>
+      <c r="Q9" s="30">
+        <v>24.928000000000001</v>
+      </c>
       <c r="T9" s="30">
         <v>28.48</v>
       </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U9" s="30">
+        <v>29.864999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B10" s="27" t="s">
         <v>88</v>
       </c>
       <c r="P10" s="30">
         <v>3.0259999999999998</v>
       </c>
+      <c r="Q10" s="30">
+        <v>4.0270000000000001</v>
+      </c>
       <c r="T10" s="30">
         <v>4.085</v>
       </c>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U10" s="30">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B11" s="27" t="s">
         <v>89</v>
       </c>
       <c r="P11" s="30">
         <v>5.726</v>
       </c>
+      <c r="Q11" s="30">
+        <v>5.8070000000000004</v>
+      </c>
       <c r="T11" s="30">
         <v>7.0679999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U11" s="30">
+        <v>8.3829999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="27" t="s">
         <v>90</v>
@@ -2461,11 +2712,17 @@
       <c r="P12" s="30">
         <v>3.0680000000000001</v>
       </c>
+      <c r="Q12" s="30">
+        <v>3.1779999999999999</v>
+      </c>
       <c r="T12" s="30">
         <v>2.3260000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U12" s="30">
+        <v>2.3460000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="28" t="s">
         <v>109</v>
@@ -2474,12 +2731,20 @@
         <f>SUM(P5:P12)</f>
         <v>273.14400000000001</v>
       </c>
+      <c r="Q13" s="30">
+        <f>SUM(Q5:Q12)</f>
+        <v>301.56100000000004</v>
+      </c>
       <c r="T13" s="30">
         <f>SUM(T5:T12)</f>
         <v>337.41800000000006</v>
       </c>
-    </row>
-    <row r="14" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U13" s="30">
+        <f>SUM(U5:U12)</f>
+        <v>343.21000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="29" t="s">
         <v>113</v>
       </c>
@@ -2487,12 +2752,20 @@
         <f>P4-P13</f>
         <v>136.72800000000001</v>
       </c>
+      <c r="Q14" s="31">
+        <f>Q4-Q13</f>
+        <v>164.39399999999995</v>
+      </c>
       <c r="T14" s="31">
         <f>T4-T13</f>
         <v>172.24999999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U14" s="31">
+        <f>U4-U13</f>
+        <v>173.70600000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>83</v>
@@ -2500,33 +2773,51 @@
       <c r="P15" s="30">
         <v>75.632999999999996</v>
       </c>
+      <c r="Q15" s="30">
+        <v>77.751000000000005</v>
+      </c>
       <c r="T15" s="30">
         <v>81.372</v>
       </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="U15" s="30">
+        <v>83.283000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>110</v>
       </c>
       <c r="P16" s="30">
         <v>14.75</v>
       </c>
+      <c r="Q16" s="30">
+        <v>17.204999999999998</v>
+      </c>
       <c r="T16" s="30">
         <v>20.361000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U16" s="30">
+        <v>17.763999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
       <c r="P17" s="30">
         <v>38.274000000000001</v>
       </c>
+      <c r="Q17" s="30">
+        <v>30.321999999999999</v>
+      </c>
       <c r="T17" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U17" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>92</v>
       </c>
@@ -2534,12 +2825,20 @@
         <f>P14-P15-P16+P17</f>
         <v>84.619000000000014</v>
       </c>
+      <c r="Q18" s="31">
+        <f>Q14-Q15-Q16+Q17</f>
+        <v>99.759999999999948</v>
+      </c>
       <c r="T18" s="31">
         <f>T14-T15-T16+T17</f>
         <v>70.516999999999939</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18" s="31">
+        <f>U14-U15-U16+U17</f>
+        <v>72.65900000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>93</v>
@@ -2547,44 +2846,68 @@
       <c r="P19" s="30">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="Q19" s="30">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="T19" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U19" s="30">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>94</v>
       </c>
       <c r="P20" s="30">
         <v>4.4560000000000004</v>
       </c>
+      <c r="Q20" s="30">
+        <v>4.4569999999999999</v>
+      </c>
       <c r="T20" s="2">
         <v>5.3879999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U20" s="30">
+        <v>4.6349999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="P21" s="30">
         <v>-6.5049999999999999</v>
       </c>
+      <c r="Q21" s="30">
+        <v>0</v>
+      </c>
       <c r="T21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U21" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
       <c r="P22" s="30">
         <v>35.703000000000003</v>
       </c>
+      <c r="Q22" s="30">
+        <v>-7.3780000000000001</v>
+      </c>
       <c r="T22" s="2">
         <v>6.0110000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U22" s="30">
+        <v>0.69499999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
         <v>97</v>
@@ -2592,11 +2915,17 @@
       <c r="P23" s="30">
         <v>0.96499999999999997</v>
       </c>
+      <c r="Q23" s="30">
+        <v>-14.459</v>
+      </c>
       <c r="T23" s="2">
         <v>-3.22</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U23" s="30">
+        <v>-12.167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>111</v>
@@ -2604,11 +2933,17 @@
       <c r="P24" s="30">
         <v>-15.021000000000001</v>
       </c>
+      <c r="Q24" s="30">
+        <v>-1.147</v>
+      </c>
       <c r="T24" s="2">
         <v>-9.4610000000000003</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U24" s="30">
+        <v>-0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>112</v>
@@ -2617,12 +2952,20 @@
         <f>P19+P20+P21+P22+P23+P24</f>
         <v>19.607000000000006</v>
       </c>
+      <c r="Q25" s="30">
+        <f>Q19+Q20+Q21+Q22+Q23+Q24</f>
+        <v>-18.518999999999998</v>
+      </c>
       <c r="T25" s="2">
         <f>T19+T20+T21+T22+T23+T24</f>
         <v>-1.2670000000000012</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U25" s="30">
+        <f>U19+U20+U21+U22+U23+U24</f>
+        <v>-7.7349999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
         <v>98</v>
       </c>
@@ -2630,23 +2973,37 @@
         <f>P18+P25</f>
         <v>104.22600000000003</v>
       </c>
+      <c r="Q26" s="30">
+        <f>Q18+Q25</f>
+        <v>81.240999999999957</v>
+      </c>
       <c r="T26" s="30">
         <f>T18+T25</f>
         <v>69.249999999999943</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U26" s="30">
+        <f>U18+U25</f>
+        <v>64.924000000000021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
         <v>99</v>
       </c>
       <c r="P27" s="30">
         <v>24.356999999999999</v>
       </c>
+      <c r="Q27" s="30">
+        <v>18.878</v>
+      </c>
       <c r="T27" s="2">
         <v>15.04</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U27" s="30">
+        <v>14.736000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
         <v>100</v>
       </c>
@@ -2654,23 +3011,37 @@
         <f>P26-P27</f>
         <v>79.869000000000028</v>
       </c>
+      <c r="Q28" s="30">
+        <f>Q26-Q27</f>
+        <v>62.362999999999957</v>
+      </c>
       <c r="T28" s="30">
         <f>T26-T27</f>
         <v>54.209999999999944</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U28" s="30">
+        <f>U26-U27</f>
+        <v>50.188000000000017</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>101</v>
       </c>
       <c r="P29" s="30">
         <v>6.5000000000000002E-2</v>
       </c>
+      <c r="Q29" s="30">
+        <v>2.3090000000000002</v>
+      </c>
       <c r="T29" s="2">
         <v>0.88200000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U29" s="30">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>102</v>
       </c>
@@ -2678,12 +3049,20 @@
         <f>P28+P29</f>
         <v>79.934000000000026</v>
       </c>
+      <c r="Q30" s="31">
+        <f>Q28+Q29</f>
+        <v>64.671999999999954</v>
+      </c>
       <c r="T30" s="31">
         <f>T28+T29</f>
         <v>55.091999999999942</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U30" s="31">
+        <f>U28+U29</f>
+        <v>51.042000000000016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B31" s="2" t="s">
         <v>103</v>
       </c>
@@ -2691,23 +3070,37 @@
         <f>P30/P32</f>
         <v>1.1719496818461723</v>
       </c>
+      <c r="Q31" s="32">
+        <f>Q30/Q32</f>
+        <v>0.87725342846678633</v>
+      </c>
       <c r="T31" s="32">
         <f>T30/T32</f>
         <v>0.74468775344687665</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U31" s="32">
+        <f>U30/U32</f>
+        <v>0.68977539933511733</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P32" s="2">
+      <c r="P32" s="32">
         <v>68.206000000000003</v>
+      </c>
+      <c r="Q32" s="32">
+        <v>73.721000000000004</v>
       </c>
       <c r="T32" s="2">
         <v>73.98</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U32" s="76">
+        <v>73.998000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26"/>
       <c r="B34" s="1" t="s">
         <v>104</v>
@@ -2716,13 +3109,21 @@
         <f>T4/P4-1</f>
         <v>0.24348089159542496</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U34" s="34">
+        <f>U4/Q4-1</f>
+        <v>0.10936893047611917</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U35" s="33">
+        <f>U4/T4-1</f>
+        <v>1.422102231256428E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B37" s="2" t="s">
         <v>106</v>
       </c>
@@ -2730,12 +3131,20 @@
         <f>P14/P4</f>
         <v>0.3335870710856072</v>
       </c>
+      <c r="Q37" s="33">
+        <f t="shared" ref="Q37" si="0">Q14/Q4</f>
+        <v>0.35281089375583469</v>
+      </c>
       <c r="T37" s="33">
         <f>T14/T4</f>
         <v>0.33796510669690843</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U37" s="33">
+        <f>U14/U4</f>
+        <v>0.33604299344574362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
         <v>107</v>
@@ -2744,12 +3153,20 @@
         <f>P18/P4</f>
         <v>0.20645225826599525</v>
       </c>
+      <c r="Q38" s="33">
+        <f t="shared" ref="Q38" si="1">Q18/Q4</f>
+        <v>0.21409792791149349</v>
+      </c>
       <c r="T38" s="33">
         <f>T18/T4</f>
         <v>0.13835869624932295</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U38" s="33">
+        <f>U18/U4</f>
+        <v>0.14056248984361097</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="20"/>
       <c r="B39" s="2" t="s">
         <v>108</v>
@@ -2758,12 +3175,20 @@
         <f>P30/P4</f>
         <v>0.19502186048327289</v>
       </c>
+      <c r="Q39" s="33">
+        <f t="shared" ref="Q39" si="2">Q30/Q4</f>
+        <v>0.13879451878400265</v>
+      </c>
       <c r="T39" s="33">
         <f>T30/T4</f>
         <v>0.10809389641884509</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U39" s="33">
+        <f>U30/U4</f>
+        <v>9.874331612873273E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B40" s="2" t="s">
         <v>99</v>
       </c>
@@ -2771,305 +3196,526 @@
         <f>P27/P26</f>
         <v>0.23369408784756196</v>
       </c>
+      <c r="Q40" s="33">
+        <f t="shared" ref="Q40" si="3">Q27/Q26</f>
+        <v>0.23237035487007804</v>
+      </c>
       <c r="T40" s="33">
         <f>T27/T26</f>
         <v>0.21718411552346586</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U40" s="33">
+        <f>U27/U26</f>
+        <v>0.22697307621218649</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="20"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B44" s="35" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="R45" s="31">
+        <v>69.495999999999995</v>
+      </c>
       <c r="T45" s="31">
         <v>47.151000000000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U45" s="31">
+        <v>54.485999999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+      <c r="R46" s="30">
+        <v>205.399</v>
       </c>
       <c r="T46" s="30">
         <v>260.26</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U46" s="30">
+        <v>250.548</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="R47" s="30">
+        <v>49.204000000000001</v>
       </c>
       <c r="T47" s="30">
         <v>54.005000000000003</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U47" s="30">
+        <v>55.322000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="R48" s="30">
+        <v>28.742000000000001</v>
       </c>
       <c r="T48" s="30">
         <v>28.157</v>
       </c>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U48" s="30">
+        <v>28.280999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+      <c r="R49" s="30">
+        <f>SUM(R45:R48)</f>
+        <v>352.84100000000001</v>
       </c>
       <c r="T49" s="30">
         <f>SUM(T45:T48)</f>
         <v>389.57299999999998</v>
       </c>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U49" s="30">
+        <f>SUM(U45:U48)</f>
+        <v>388.637</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="R50" s="30">
+        <v>2129.9340000000002</v>
       </c>
       <c r="T50" s="30">
         <v>2270.6559999999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U50" s="30">
+        <v>2339.2779999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B51" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="R51" s="30">
+        <v>102.913</v>
       </c>
       <c r="T51" s="30">
         <v>91.293000000000006</v>
       </c>
-    </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U51" s="30">
+        <v>85.471999999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B52" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="R52" s="30">
+        <v>505.125</v>
       </c>
       <c r="T52" s="30">
         <v>498.07299999999998</v>
       </c>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U52" s="30">
+        <v>495.19499999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B53" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="R53" s="30">
+        <v>62.643999999999998</v>
       </c>
       <c r="T53" s="30">
         <v>64.155000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U53" s="30">
+        <v>61.741999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B54" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+      <c r="R54" s="30">
+        <v>113.878</v>
       </c>
       <c r="T54" s="30">
         <v>145.80000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U54" s="30">
+        <v>154.84100000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B55" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="R55" s="30">
+        <f>R49+SUM(R50:R54)</f>
+        <v>3267.335</v>
       </c>
       <c r="T55" s="30">
         <f>T49+SUM(T50:T54)</f>
         <v>3459.55</v>
       </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U55" s="30">
+        <f>U49+SUM(U50:U54)</f>
+        <v>3525.1650000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="R56" s="30"/>
       <c r="T56" s="30"/>
     </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B57" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="R57" s="30">
+        <v>174.23699999999999</v>
       </c>
       <c r="T57" s="30">
         <v>194.95099999999999</v>
       </c>
-    </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U57" s="30">
+        <v>186.46</v>
+      </c>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B58" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="R58" s="30">
+        <v>56.652000000000001</v>
       </c>
       <c r="T58" s="30">
         <v>62.537999999999997</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U58" s="30">
+        <v>60.17</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B59" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="R59" s="30">
+        <v>14.95</v>
       </c>
       <c r="T59" s="30">
         <v>11.423</v>
       </c>
-    </row>
-    <row r="60" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U59" s="30">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="R60" s="31">
+        <v>0.628</v>
       </c>
       <c r="T60" s="31">
         <v>0.63400000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U60" s="31">
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B61" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="R61" s="30">
+        <v>18.783000000000001</v>
       </c>
       <c r="T61" s="30">
         <v>20.497</v>
       </c>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U61" s="30">
+        <v>21.879000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B62" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="R62" s="30">
+        <v>47.381</v>
       </c>
       <c r="T62" s="30">
         <v>38.292999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U62" s="30">
+        <v>37.289000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B63" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="R63" s="30">
+        <f>SUM(R57:R62)</f>
+        <v>312.63099999999997</v>
       </c>
       <c r="T63" s="30">
         <f>SUM(T57:T62)</f>
         <v>328.33600000000001</v>
       </c>
-    </row>
-    <row r="64" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U63" s="30">
+        <f>SUM(U57:U62)</f>
+        <v>319.34500000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="R64" s="31">
+        <v>1298.7349999999999</v>
       </c>
       <c r="T64" s="31">
         <v>1358.8420000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U64" s="31">
+        <v>1369.0060000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="R65" s="30">
+        <v>0.91500000000000004</v>
       </c>
       <c r="T65" s="30">
         <v>0.85099999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U65" s="30">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="R66" s="30">
+        <v>21.337</v>
       </c>
       <c r="T66" s="30">
         <v>20.375</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U66" s="30">
+        <v>20.14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B67" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="R67" s="30">
+        <v>44.387</v>
       </c>
       <c r="T67" s="30">
         <v>44.305</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U67" s="30">
+        <v>40.581000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B68" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="R68" s="30">
+        <v>49.661999999999999</v>
       </c>
       <c r="T68" s="30">
         <v>53.595999999999997</v>
       </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U68" s="30">
+        <v>56.81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B69" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="R69" s="30">
+        <v>217.291</v>
       </c>
       <c r="T69" s="30">
         <v>241.75200000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U69" s="30">
+        <v>253.036</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B70" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="R70" s="30">
+        <f>R63+SUM(R64:R69)</f>
+        <v>1944.9579999999996</v>
       </c>
       <c r="T70" s="30">
         <f>T63+SUM(T64:T69)</f>
         <v>2048.0570000000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U70" s="30">
+        <f>U63+SUM(U64:U69)</f>
+        <v>2059.6329999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B72" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="R72" s="30">
+        <v>1322.377</v>
       </c>
       <c r="T72" s="30">
         <v>1411.4929999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U72" s="30">
+        <v>1465.5319999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B73" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="R73" s="30">
+        <f>R72+R70</f>
+        <v>3267.3349999999996</v>
       </c>
       <c r="T73" s="30">
         <f>T72+T70</f>
         <v>3459.55</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U73" s="30">
+        <f>U72+U70</f>
+        <v>3525.165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B75" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="R75" s="30">
+        <f>R55-R70</f>
+        <v>1322.3770000000004</v>
       </c>
       <c r="T75" s="30">
         <f>T55-T70</f>
         <v>1411.4929999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U75" s="30">
+        <f t="shared" ref="U75" si="4">U55-U70</f>
+        <v>1465.5320000000006</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A76" s="20"/>
       <c r="B76" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="R76" s="70"/>
       <c r="T76" s="2">
         <f>T75/T32</f>
         <v>19.079386320627194</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U76" s="2">
+        <f t="shared" ref="U76" si="5">U75/U32</f>
+        <v>19.8050217573448</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A77" s="20"/>
     </row>
-    <row r="78" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B78" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="T78" s="46">
+      <c r="R78" s="44">
+        <f>R45</f>
+        <v>69.495999999999995</v>
+      </c>
+      <c r="T78" s="44">
         <f>T45</f>
         <v>47.151000000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U78" s="44">
+        <f t="shared" ref="U78" si="6">U45</f>
+        <v>54.485999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B79" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="T79" s="46">
+      <c r="R79" s="44">
+        <f>R60+R64</f>
+        <v>1299.3629999999998</v>
+      </c>
+      <c r="T79" s="44">
         <f>T60+T64</f>
         <v>1359.4760000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U79" s="44">
+        <f t="shared" ref="U79" si="7">U60+U64</f>
+        <v>1369.643</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B80" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="R80" s="30">
+        <f>R78-R79</f>
+        <v>-1229.8669999999997</v>
       </c>
       <c r="T80" s="30">
         <f>T78-T79</f>
         <v>-1312.325</v>
       </c>
-    </row>
-    <row r="82" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U80" s="30">
+        <f t="shared" ref="U80" si="8">U78-U79</f>
+        <v>-1315.1569999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B82" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T82" s="2">
         <v>28.73</v>
       </c>
-    </row>
-    <row r="83" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U82" s="2">
+        <v>24.09</v>
+      </c>
+    </row>
+    <row r="83" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B83" s="2" t="s">
         <v>5</v>
       </c>
@@ -3077,8 +3723,12 @@
         <f>T82*T32</f>
         <v>2125.4454000000001</v>
       </c>
-    </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U83" s="30">
+        <f t="shared" ref="U83" si="9">U82*U32</f>
+        <v>1782.6118200000001</v>
+      </c>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B84" s="2" t="s">
         <v>9</v>
       </c>
@@ -3086,27 +3736,35 @@
         <f>T83-T80</f>
         <v>3437.7704000000003</v>
       </c>
-    </row>
-    <row r="86" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U84" s="30">
+        <f t="shared" ref="U84" si="10">U83-U80</f>
+        <v>3097.7688200000002</v>
+      </c>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B86" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T86" s="45">
+      <c r="T86" s="43">
         <f>T82/T76</f>
         <v>1.5058136313818067</v>
       </c>
-    </row>
-    <row r="87" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U86" s="43">
+        <f t="shared" ref="U86" si="11">U82/U76</f>
+        <v>1.2163581689106751</v>
+      </c>
+    </row>
+    <row r="87" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B87" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B88" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B89" s="2" t="s">
         <v>30</v>
       </c>
@@ -3114,11 +3772,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T1" r:id="rId1" xr:uid="{228CD04C-DFDD-4929-9CEF-C123195CA26C}"/>
+    <hyperlink ref="U1" r:id="rId2" xr:uid="{39BB2612-7FA1-4444-8959-CB6DC57927E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="T13 P13" formulaRange="1"/>
+    <ignoredError sqref="T13:U13 P13:Q13" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>